<commit_message>
adding weighted and non-weighted graphing options
</commit_message>
<xml_diff>
--- a/popvsflower.xlsx
+++ b/popvsflower.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\Documents\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\Documents\R\github\flowerandpopcorn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0364CC89-72ED-4F5A-ADBD-FD59250D00F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8832851-4540-4B98-B83E-D2834031790A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9E8440D5-C1CE-4DB6-A598-F42C76F18A6F}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId3"/>
+    <pivotCache cacheId="33" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -254,6 +254,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -305,17 +308,23 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="164" formatCode="0.00000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="164" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
       <font>
@@ -334,12 +343,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
       <font>
@@ -15350,7 +15353,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D809ADF6-D0F8-40F3-A41E-8B0792D1E900}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D809ADF6-D0F8-40F3-A41E-8B0792D1E900}" name="PivotTable1" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:E212" firstHeaderRow="1" firstDataRow="2" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="15">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -16226,7 +16229,7 @@
     <sortCondition ref="A4:A146"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{EF080A29-D767-42CB-8C21-22C107A9B0C5}" name="harvest" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{EF080A29-D767-42CB-8C21-22C107A9B0C5}" name="harvest" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{1F40EEFD-1A7C-4993-A796-494A1152DA1E}" name="strain"/>
     <tableColumn id="3" xr3:uid="{0B704505-CEB4-4865-8ADF-AD6D6EC8F3EA}" name="flower" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{E0538822-C362-400E-BC79-87B8983E3B4A}" name="popcorn" dataDxfId="0"/>
@@ -16242,10 +16245,10 @@
     <sortCondition ref="I4:I146"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A0C6862A-3125-474B-AA87-9EB9F244E8C9}" name="Harvest" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{A0C6862A-3125-474B-AA87-9EB9F244E8C9}" name="Harvest" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{6402A35A-B553-42B7-8E09-60B73EE2AD07}" name="Strain"/>
-    <tableColumn id="3" xr3:uid="{97624292-B4E6-4470-974B-9433A4425CDC}" name="Flower %" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{F077FAC9-2B3B-4B81-91B8-82C9BC48EAD3}" name="Popcorn %" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{97624292-B4E6-4470-974B-9433A4425CDC}" name="Flower %" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{F077FAC9-2B3B-4B81-91B8-82C9BC48EAD3}" name="Popcorn %" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -16551,7 +16554,7 @@
   <dimension ref="A1:D143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I13:I14"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>